<commit_message>
Fix formatting of lut_generator_rid.xlsx
</commit_message>
<xml_diff>
--- a/lut_generator_rid.xlsx
+++ b/lut_generator_rid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shared\Dokumente\codebase\avr-rid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E4FE97-35C1-485B-8F82-D2D7D85C69A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B815C9AF-E09C-4F92-97D5-BA012690DF83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9730" yWindow="0" windowWidth="36500" windowHeight="18320" xr2:uid="{F31E432E-1247-4F18-8B99-AC2EE1672703}"/>
+    <workbookView xWindow="10690" yWindow="0" windowWidth="36500" windowHeight="18320" xr2:uid="{F31E432E-1247-4F18-8B99-AC2EE1672703}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -437,6 +437,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -458,7 +461,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -790,7 +793,7 @@
   <dimension ref="A1:R48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+      <selection activeCell="F35" sqref="F5:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -810,29 +813,29 @@
     <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="24" t="s">
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="24" t="s">
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="9"/>
@@ -885,10 +888,10 @@
     <row r="5" spans="1:16" s="9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="13"/>
       <c r="C5" s="14"/>
-      <c r="E5" s="27">
+      <c r="E5" s="20">
         <v>0</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="28">
         <v>685.23646008640594</v>
       </c>
       <c r="G5" s="10">
@@ -916,15 +919,15 @@
         <v>0</v>
       </c>
       <c r="M5" s="7" t="str">
-        <f>IF(L5&lt;&gt;"",L5+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" ref="M5:M33" si="0">IF(L5&lt;&gt;"",L5+COUNT(L:L)&amp;", ","")</f>
         <v xml:space="preserve">10, </v>
       </c>
       <c r="N5" s="18" t="str">
-        <f t="shared" ref="N5:N33" si="0">IF(J5&lt;&gt;"",J5-1&amp;", "&amp;IF($H5&lt;&gt;$H6,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
+        <f t="shared" ref="N5:N33" si="1">IF(J5&lt;&gt;"",J5-1&amp;", "&amp;IF($H5&lt;&gt;$H6,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
         <v xml:space="preserve">20, </v>
       </c>
       <c r="O5" s="18"/>
-      <c r="P5" s="21" t="str">
+      <c r="P5" s="22" t="str">
         <f>"const __flash uint"&amp;$C$8*8&amp;"_t "&amp;"lut"&amp;$C$7*8&amp;"_"&amp;$C$6&amp;"["&amp;COUNT($J:$J)+1+COUNT($L:$L)&amp;"] ="&amp;CHAR(10)&amp;"{"&amp;CHAR(10)&amp;_xlfn.CONCAT($M:$M)&amp;CHAR(10)&amp;CHAR(10)&amp;_xlfn.CONCAT($N:$N)&amp;"};"</f>
         <v>const __flash uint8_t lut16_rid[42] =
 {
@@ -953,46 +956,46 @@
         <v>21</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="27">
+      <c r="E6" s="20">
         <v>1000</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="28">
         <v>1259.2978106741325</v>
       </c>
       <c r="G6" s="10">
-        <f t="shared" ref="G6:G35" si="1">F6/(2^$C$13)</f>
+        <f t="shared" ref="G6:G35" si="2">F6/(2^$C$13)</f>
         <v>39.353056583566641</v>
       </c>
       <c r="H6" s="6">
-        <f t="shared" ref="H6:H35" si="2">IF(CEILING(LOG(G6+1,2),1)&lt;$C$8*8,$C$8*8,CEILING(LOG(G6+1,2),1))</f>
+        <f t="shared" ref="H6:H35" si="3">IF(CEILING(LOG(G6+1,2),1)&lt;$C$8*8,$C$8*8,CEILING(LOG(G6+1,2),1))</f>
         <v>8</v>
       </c>
       <c r="I6" s="10">
-        <f t="shared" ref="I6:I35" si="3">G6/2^(H6-($C$8*8))</f>
+        <f t="shared" ref="I6:I35" si="4">G6/2^(H6-($C$8*8))</f>
         <v>39.353056583566641</v>
       </c>
       <c r="J6" s="15">
-        <f t="shared" ref="J6:J35" si="4">ROUND(I6,0)</f>
+        <f t="shared" ref="J6:J35" si="5">ROUND(I6,0)</f>
         <v>39</v>
       </c>
       <c r="K6" s="16">
-        <f t="shared" ref="K6:K35" si="5">I6/J6-1</f>
+        <f t="shared" ref="K6:K35" si="6">I6/J6-1</f>
         <v>9.0527329119651778E-3</v>
       </c>
       <c r="L6" s="6" t="str">
-        <f t="shared" ref="L6:L9" si="6">IF($H5&lt;&gt;$H6,ROW($H6)-ROW($H$5),"")</f>
+        <f t="shared" ref="L6:L9" si="7">IF($H5&lt;&gt;$H6,ROW($H6)-ROW($H$5),"")</f>
         <v/>
       </c>
       <c r="M6" s="7" t="str">
-        <f>IF(L6&lt;&gt;"",L6+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N6" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">38, </v>
       </c>
       <c r="O6" s="18"/>
-      <c r="P6" s="22"/>
+      <c r="P6" s="23"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
@@ -1003,46 +1006,46 @@
         <v>2</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="27">
+      <c r="E7" s="20">
         <v>1500</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="28">
         <v>1871.6732435999043</v>
       </c>
       <c r="G7" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58.489788862497008</v>
       </c>
       <c r="H7" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I7" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>58.489788862497008</v>
       </c>
       <c r="J7" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>58</v>
       </c>
       <c r="K7" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.4446355602931789E-3</v>
       </c>
       <c r="L7" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="M7" s="7" t="str">
-        <f>IF(L7&lt;&gt;"",L7+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N7" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">57, </v>
       </c>
       <c r="O7" s="18"/>
-      <c r="P7" s="22"/>
+      <c r="P7" s="23"/>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
@@ -1053,46 +1056,46 @@
         <v>1</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="27">
+      <c r="E8" s="20">
         <v>2200</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="28">
         <v>2815.422909869797</v>
       </c>
       <c r="G8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>87.981965933431155</v>
       </c>
       <c r="H8" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I8" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87.981965933431155</v>
       </c>
       <c r="J8" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>88</v>
       </c>
       <c r="K8" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-2.0493257464593295E-4</v>
       </c>
       <c r="L8" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="M8" s="7" t="str">
-        <f>IF(L8&lt;&gt;"",L8+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N8" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">87, </v>
       </c>
       <c r="O8" s="18"/>
-      <c r="P8" s="22"/>
+      <c r="P8" s="23"/>
     </row>
     <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
@@ -1103,187 +1106,187 @@
         <v>16</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="27">
+      <c r="E9" s="20">
         <v>3300</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="28">
         <v>4060.6442006114239</v>
       </c>
       <c r="G9" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>126.895131269107</v>
       </c>
       <c r="H9" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I9" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>126.895131269107</v>
       </c>
       <c r="J9" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>127</v>
       </c>
       <c r="K9" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-8.2573803852759031E-4</v>
       </c>
       <c r="L9" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="M9" s="7" t="str">
-        <f>IF(L9&lt;&gt;"",L9+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N9" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">126, </v>
       </c>
       <c r="O9" s="18"/>
-      <c r="P9" s="22"/>
+      <c r="P9" s="23"/>
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="3"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="27">
+      <c r="E10" s="20">
         <v>4700</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="28">
         <v>5007.8360248450799</v>
       </c>
       <c r="G10" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>156.49487577640875</v>
       </c>
       <c r="H10" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I10" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>156.49487577640875</v>
       </c>
       <c r="J10" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>156</v>
       </c>
       <c r="K10" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.1722806180047858E-3</v>
       </c>
       <c r="L10" s="6" t="str">
-        <f t="shared" ref="L10:L33" si="7">IF($H9&lt;&gt;$H10,ROW($H10)-ROW($H$5),"")</f>
+        <f t="shared" ref="L10:L33" si="8">IF($H9&lt;&gt;$H10,ROW($H10)-ROW($H$5),"")</f>
         <v/>
       </c>
       <c r="M10" s="7" t="str">
-        <f>IF(L10&lt;&gt;"",L10+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N10" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">155, </v>
       </c>
       <c r="O10" s="18"/>
-      <c r="P10" s="22"/>
+      <c r="P10" s="23"/>
     </row>
     <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="3"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="27">
+      <c r="E11" s="20">
         <v>5600</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="28">
         <v>6066.491407791038</v>
       </c>
       <c r="G11" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>189.57785649346994</v>
       </c>
       <c r="H11" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I11" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>189.57785649346994</v>
       </c>
       <c r="J11" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
       <c r="K11" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-2.2218079291056458E-3</v>
       </c>
       <c r="L11" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M11" s="7" t="str">
-        <f>IF(L11&lt;&gt;"",L11+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N11" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">189, </v>
       </c>
       <c r="O11" s="18"/>
-      <c r="P11" s="22"/>
+      <c r="P11" s="23"/>
     </row>
     <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="27">
+      <c r="E12" s="20">
         <v>6800</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="28">
         <v>7332.8697462109321</v>
       </c>
       <c r="G12" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>229.15217956909163</v>
       </c>
       <c r="H12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I12" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>229.15217956909163</v>
       </c>
       <c r="J12" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>229</v>
       </c>
       <c r="K12" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.6453960302026438E-4</v>
       </c>
       <c r="L12" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M12" s="7" t="str">
-        <f>IF(L12&lt;&gt;"",L12+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N12" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">228, 
 </v>
       </c>
       <c r="O12" s="18"/>
-      <c r="P12" s="22"/>
+      <c r="P12" s="23"/>
     </row>
     <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
@@ -1295,144 +1298,144 @@
         <v>5</v>
       </c>
       <c r="D13" s="7"/>
-      <c r="E13" s="27">
+      <c r="E13" s="20">
         <v>8200</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="28">
         <v>8930.763873817019</v>
       </c>
       <c r="G13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>279.08637105678184</v>
       </c>
       <c r="H13" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="I13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>139.54318552839092</v>
       </c>
       <c r="J13" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>140</v>
       </c>
       <c r="K13" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-3.2629605114934401E-3</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="M13" s="7" t="str">
-        <f>IF(L13&lt;&gt;"",L13+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">18, </v>
       </c>
       <c r="N13" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">139, </v>
       </c>
       <c r="O13" s="18"/>
-      <c r="P13" s="22"/>
+      <c r="P13" s="23"/>
     </row>
     <row r="14" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
       <c r="B14" s="3"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="27">
+      <c r="E14" s="20">
         <v>10000</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="28">
         <v>10757.547785526249</v>
       </c>
       <c r="G14" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>336.17336829769528</v>
       </c>
       <c r="H14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>168.08668414884764</v>
       </c>
       <c r="J14" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="K14" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.159770764739946E-4</v>
       </c>
       <c r="L14" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M14" s="7" t="str">
-        <f>IF(L14&lt;&gt;"",L14+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N14" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">167, </v>
       </c>
       <c r="O14" s="18"/>
-      <c r="P14" s="22"/>
+      <c r="P14" s="23"/>
     </row>
     <row r="15" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="20"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="27">
+      <c r="E15" s="20">
         <v>12000</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="28">
         <v>13348.183903720461</v>
       </c>
       <c r="G15" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>417.1307469912644</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="I15" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>208.5653734956322</v>
       </c>
       <c r="J15" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>209</v>
       </c>
       <c r="K15" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-2.079552652477501E-3</v>
       </c>
       <c r="L15" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M15" s="7" t="str">
-        <f>IF(L15&lt;&gt;"",L15+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N15" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">208, </v>
       </c>
       <c r="O15" s="18"/>
-      <c r="P15" s="22"/>
+      <c r="P15" s="23"/>
     </row>
     <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
-      <c r="B16" s="23" t="str">
+      <c r="B16" s="24" t="str">
         <f>$P$5</f>
         <v>const __flash uint8_t lut16_rid[42] =
 {
@@ -1451,836 +1454,836 @@
 255
 };</v>
       </c>
-      <c r="C16" s="23"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="27">
+      <c r="E16" s="20">
         <v>15000</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="28">
         <v>16151.90067355656</v>
       </c>
       <c r="G16" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>504.7468960486425</v>
       </c>
       <c r="H16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="I16" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>252.37344802432125</v>
       </c>
       <c r="J16" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>252</v>
       </c>
       <c r="K16" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4819366044493965E-3</v>
       </c>
       <c r="L16" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M16" s="7" t="str">
-        <f>IF(L16&lt;&gt;"",L16+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N16" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">251, 
 </v>
       </c>
       <c r="O16" s="18"/>
-      <c r="P16" s="22"/>
+      <c r="P16" s="23"/>
     </row>
     <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="3"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="27">
+      <c r="E17" s="20">
         <v>18000</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="28">
         <v>19675.378577762247</v>
       </c>
       <c r="G17" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>614.85558055507022</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="I17" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>153.71389513876755</v>
       </c>
       <c r="J17" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>154</v>
       </c>
       <c r="K17" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.857823774236711E-3</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="M17" s="7" t="str">
-        <f>IF(L17&lt;&gt;"",L17+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">22, </v>
       </c>
       <c r="N17" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">153, </v>
       </c>
       <c r="O17" s="18"/>
-      <c r="P17" s="22"/>
+      <c r="P17" s="23"/>
     </row>
     <row r="18" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="27">
+      <c r="E18" s="20">
         <v>22000</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="28">
         <v>24131.245905036554</v>
       </c>
       <c r="G18" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>754.10143453239232</v>
       </c>
       <c r="H18" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="I18" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>188.52535863309808</v>
       </c>
       <c r="J18" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>189</v>
       </c>
       <c r="K18" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-2.5113299836080349E-3</v>
       </c>
       <c r="L18" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M18" s="7" t="str">
-        <f>IF(L18&lt;&gt;"",L18+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N18" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">188, </v>
       </c>
       <c r="O18" s="18"/>
-      <c r="P18" s="22"/>
+      <c r="P18" s="23"/>
     </row>
     <row r="19" spans="1:16" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
       <c r="B19" s="3"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="27">
+      <c r="E19" s="20">
         <v>27000</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="28">
         <v>29519.529890767029</v>
       </c>
       <c r="G19" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>922.48530908646967</v>
       </c>
       <c r="H19" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="I19" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>230.62132727161742</v>
       </c>
       <c r="J19" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>231</v>
       </c>
       <c r="K19" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.6392758804441021E-3</v>
       </c>
       <c r="L19" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M19" s="7" t="str">
-        <f>IF(L19&lt;&gt;"",L19+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N19" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">230, 
 </v>
       </c>
       <c r="O19" s="18"/>
-      <c r="P19" s="22"/>
+      <c r="P19" s="23"/>
     </row>
     <row r="20" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
       <c r="B20" s="3"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="27">
+      <c r="E20" s="20">
         <v>33000</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="28">
         <v>35121.328844124095</v>
       </c>
       <c r="G20" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1097.541526378878</v>
       </c>
       <c r="H20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>137.19269079735975</v>
       </c>
       <c r="J20" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>137</v>
       </c>
       <c r="K20" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.406502170509194E-3</v>
       </c>
       <c r="L20" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="M20" s="7" t="str">
-        <f>IF(L20&lt;&gt;"",L20+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">25, </v>
       </c>
       <c r="N20" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">136, </v>
       </c>
       <c r="O20" s="18"/>
-      <c r="P20" s="22"/>
+      <c r="P20" s="23"/>
     </row>
     <row r="21" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
       <c r="B21" s="3"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="27">
+      <c r="E21" s="20">
         <v>39000</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="28">
         <v>42156.601554598208</v>
       </c>
       <c r="G21" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1317.393798581194</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="I21" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>164.67422482264925</v>
       </c>
       <c r="J21" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>165</v>
       </c>
       <c r="K21" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.9743950142470101E-3</v>
       </c>
       <c r="L21" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M21" s="7" t="str">
-        <f>IF(L21&lt;&gt;"",L21+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N21" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">164, </v>
       </c>
       <c r="O21" s="18"/>
-      <c r="P21" s="22"/>
+      <c r="P21" s="23"/>
     </row>
     <row r="22" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
       <c r="B22" s="3"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="27">
+      <c r="E22" s="20">
         <v>47000</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F22" s="28">
         <v>50336.199900242318</v>
       </c>
       <c r="G22" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1573.0062468825724</v>
       </c>
       <c r="H22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="I22" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>196.62578086032156</v>
       </c>
       <c r="J22" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>197</v>
       </c>
       <c r="K22" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.8995895415149233E-3</v>
       </c>
       <c r="L22" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M22" s="7" t="str">
-        <f>IF(L22&lt;&gt;"",L22+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N22" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">196, </v>
       </c>
       <c r="O22" s="18"/>
-      <c r="P22" s="22"/>
+      <c r="P22" s="23"/>
     </row>
     <row r="23" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
       <c r="B23" s="3"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="27">
+      <c r="E23" s="20">
         <v>56000</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F23" s="28">
         <v>60872.38880949279</v>
       </c>
       <c r="G23" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1902.2621502966497</v>
       </c>
       <c r="H23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="I23" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>237.78276878708121</v>
       </c>
       <c r="J23" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>238</v>
       </c>
       <c r="K23" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-9.1273618873444207E-4</v>
       </c>
       <c r="L23" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M23" s="7" t="str">
-        <f>IF(L23&lt;&gt;"",L23+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N23" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">237, 
 </v>
       </c>
       <c r="O23" s="18"/>
-      <c r="P23" s="22"/>
+      <c r="P23" s="23"/>
     </row>
     <row r="24" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
       <c r="B24" s="3"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="27">
+      <c r="E24" s="20">
         <v>68000</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="28">
         <v>73481.638335108626</v>
       </c>
       <c r="G24" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2296.3011979721446</v>
       </c>
       <c r="H24" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="I24" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>143.51882487325904</v>
       </c>
       <c r="J24" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>144</v>
       </c>
       <c r="K24" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-3.3414939357011564E-3</v>
       </c>
       <c r="L24" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="M24" s="7" t="str">
-        <f>IF(L24&lt;&gt;"",L24+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">29, </v>
       </c>
       <c r="N24" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">143, </v>
       </c>
       <c r="O24" s="18"/>
-      <c r="P24" s="22"/>
+      <c r="P24" s="23"/>
     </row>
     <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
       <c r="B25" s="3"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="27">
+      <c r="E25" s="20">
         <v>82000</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F25" s="28">
         <v>89361.283690993354</v>
       </c>
       <c r="G25" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2792.5401153435423</v>
       </c>
       <c r="H25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="I25" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>174.53375720897139</v>
       </c>
       <c r="J25" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="K25" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-2.6642445201634501E-3</v>
       </c>
       <c r="L25" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M25" s="7" t="str">
-        <f>IF(L25&lt;&gt;"",L25+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N25" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">174, </v>
       </c>
       <c r="O25" s="18"/>
-      <c r="P25" s="22"/>
+      <c r="P25" s="23"/>
     </row>
     <row r="26" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7"/>
       <c r="B26" s="3"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="27">
+      <c r="E26" s="20">
         <v>100000</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="28">
         <v>107524.32124403358</v>
       </c>
       <c r="G26" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3360.1350388760493</v>
       </c>
       <c r="H26" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="I26" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>210.00843992975308</v>
       </c>
       <c r="J26" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>210</v>
       </c>
       <c r="K26" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.0190141681328839E-5</v>
       </c>
       <c r="L26" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M26" s="7" t="str">
-        <f>IF(L26&lt;&gt;"",L26+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N26" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">209, 
 </v>
       </c>
       <c r="O26" s="18"/>
-      <c r="P26" s="22"/>
+      <c r="P26" s="23"/>
     </row>
     <row r="27" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7"/>
       <c r="B27" s="3"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="27">
+      <c r="E27" s="20">
         <v>120000</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="28">
         <v>133157.43740246791</v>
       </c>
       <c r="G27" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4161.1699188271223</v>
       </c>
       <c r="H27" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="I27" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>130.03655996334757</v>
       </c>
       <c r="J27" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>130</v>
       </c>
       <c r="K27" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.8123048728900812E-4</v>
       </c>
       <c r="L27" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="M27" s="7" t="str">
-        <f>IF(L27&lt;&gt;"",L27+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">32, </v>
       </c>
       <c r="N27" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">129, </v>
       </c>
       <c r="O27" s="18"/>
-      <c r="P27" s="22"/>
+      <c r="P27" s="23"/>
     </row>
     <row r="28" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7"/>
       <c r="B28" s="3"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="27">
+      <c r="E28" s="20">
         <v>150000</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="28">
         <v>160992.45247626147</v>
       </c>
       <c r="G28" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5031.0141398831711</v>
       </c>
       <c r="H28" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="I28" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>157.2191918713491</v>
       </c>
       <c r="J28" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>157</v>
       </c>
       <c r="K28" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3961265691024849E-3</v>
       </c>
       <c r="L28" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M28" s="7" t="str">
-        <f>IF(L28&lt;&gt;"",L28+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N28" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">156, </v>
       </c>
       <c r="O28" s="18"/>
-      <c r="P28" s="22"/>
+      <c r="P28" s="23"/>
     </row>
     <row r="29" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7"/>
       <c r="B29" s="3"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="27">
+      <c r="E29" s="20">
         <v>180000</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="28">
         <v>195782.89084646633</v>
       </c>
       <c r="G29" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6118.2153389520727</v>
       </c>
       <c r="H29" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="I29" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>191.19422934225227</v>
       </c>
       <c r="J29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>191</v>
       </c>
       <c r="K29" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0169075510590986E-3</v>
       </c>
       <c r="L29" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M29" s="7" t="str">
-        <f>IF(L29&lt;&gt;"",L29+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N29" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">190, </v>
       </c>
       <c r="O29" s="18"/>
-      <c r="P29" s="22"/>
+      <c r="P29" s="23"/>
     </row>
     <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
       <c r="B30" s="3"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
-      <c r="E30" s="27">
+      <c r="E30" s="20">
         <v>220000</v>
       </c>
-      <c r="F30" s="27">
+      <c r="F30" s="28">
         <v>239697.59388508165</v>
       </c>
       <c r="G30" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7490.5498089088014</v>
       </c>
       <c r="H30" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="I30" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>234.07968152840004</v>
       </c>
       <c r="J30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>234</v>
       </c>
       <c r="K30" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.405193521368588E-4</v>
       </c>
       <c r="L30" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M30" s="7" t="str">
-        <f>IF(L30&lt;&gt;"",L30+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N30" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">233, 
 </v>
       </c>
       <c r="O30" s="18"/>
-      <c r="P30" s="22"/>
+      <c r="P30" s="23"/>
     </row>
     <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="7"/>
       <c r="B31" s="3"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="27">
+      <c r="E31" s="20">
         <v>270000</v>
       </c>
-      <c r="F31" s="27">
+      <c r="F31" s="28">
         <v>292662.62817106448</v>
       </c>
       <c r="G31" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9145.7071303457651</v>
       </c>
       <c r="H31" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="I31" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>142.90167391165258</v>
       </c>
       <c r="J31" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>143</v>
       </c>
       <c r="K31" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-6.8759502340853818E-4</v>
       </c>
       <c r="L31" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="M31" s="7" t="str">
-        <f>IF(L31&lt;&gt;"",L31+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">36, </v>
       </c>
       <c r="N31" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">142, </v>
       </c>
       <c r="O31" s="18"/>
-      <c r="P31" s="22"/>
+      <c r="P31" s="23"/>
     </row>
     <row r="32" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7"/>
       <c r="B32" s="3"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="27">
+      <c r="E32" s="20">
         <v>330000</v>
       </c>
-      <c r="F32" s="27">
+      <c r="F32" s="28">
         <v>401391.45114954695</v>
       </c>
       <c r="G32" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12543.482848423342</v>
       </c>
       <c r="H32" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="I32" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>195.99191950661472</v>
       </c>
       <c r="J32" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>196</v>
       </c>
       <c r="K32" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-4.1227007067767829E-5</v>
       </c>
       <c r="L32" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="M32" s="7" t="str">
-        <f>IF(L32&lt;&gt;"",L32+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N32" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">195, 
 </v>
       </c>
       <c r="O32" s="18"/>
-      <c r="P32" s="22"/>
+      <c r="P32" s="23"/>
     </row>
     <row r="33" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
       <c r="B33" s="3"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
-      <c r="E33" s="27">
+      <c r="E33" s="20">
         <v>470000</v>
       </c>
-      <c r="F33" s="27">
+      <c r="F33" s="28">
         <v>574870.38618262182</v>
       </c>
       <c r="G33" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17964.699568206932</v>
       </c>
       <c r="H33" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="I33" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>140.34921537661666</v>
       </c>
       <c r="J33" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>140</v>
       </c>
       <c r="K33" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.4943955472618295E-3</v>
       </c>
       <c r="L33" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
       <c r="M33" s="7" t="str">
-        <f>IF(L33&lt;&gt;"",L33+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">38, </v>
       </c>
       <c r="N33" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">139, </v>
       </c>
       <c r="O33" s="18"/>
-      <c r="P33" s="22"/>
+      <c r="P33" s="23"/>
       <c r="R33" s="19"/>
     </row>
     <row r="34" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2288,94 +2291,94 @@
       <c r="B34" s="3"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="27">
+      <c r="E34" s="20">
         <v>680000</v>
       </c>
-      <c r="F34" s="27">
+      <c r="F34" s="28">
         <v>834047.7599130437</v>
       </c>
       <c r="G34" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26063.992497282616</v>
       </c>
       <c r="H34" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="I34" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>203.62494138502043</v>
       </c>
       <c r="J34" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>204</v>
       </c>
       <c r="K34" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.8385226224488793E-3</v>
       </c>
       <c r="L34" s="6" t="str">
-        <f t="shared" ref="L34:L36" si="8">IF($H33&lt;&gt;$H34,ROW($H34)-ROW($H$5),"")</f>
+        <f t="shared" ref="L34:L36" si="9">IF($H33&lt;&gt;$H34,ROW($H34)-ROW($H$5),"")</f>
         <v/>
       </c>
       <c r="M34" s="7" t="str">
-        <f t="shared" ref="M34:M36" si="9">IF(L34&lt;&gt;"",L34+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" ref="M34:M36" si="10">IF(L34&lt;&gt;"",L34+COUNT(L:L)&amp;", ","")</f>
         <v/>
       </c>
       <c r="N34" s="18" t="str">
-        <f t="shared" ref="N34:N36" si="10">IF(J34&lt;&gt;"",J34-1&amp;", "&amp;IF($H34&lt;&gt;$H35,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
+        <f t="shared" ref="N34:N36" si="11">IF(J34&lt;&gt;"",J34-1&amp;", "&amp;IF($H34&lt;&gt;$H35,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
         <v xml:space="preserve">203, 
 </v>
       </c>
       <c r="O34" s="18"/>
-      <c r="P34" s="22"/>
+      <c r="P34" s="23"/>
     </row>
     <row r="35" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
       <c r="B35" s="3"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="27">
+      <c r="E35" s="20">
         <v>1000000</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F35" s="28">
         <v>1394768.1263387096</v>
       </c>
       <c r="G35" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43586.503948084675</v>
       </c>
       <c r="H35" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="I35" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>170.25978104720576</v>
       </c>
       <c r="J35" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>170</v>
       </c>
       <c r="K35" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5281238070927738E-3</v>
       </c>
       <c r="L35" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="M35" s="7" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">40, </v>
       </c>
       <c r="N35" s="18" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">169, 
 </v>
       </c>
       <c r="O35" s="18"/>
-      <c r="P35" s="22"/>
+      <c r="P35" s="23"/>
     </row>
     <row r="36" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
@@ -2390,20 +2393,20 @@
       <c r="J36"/>
       <c r="K36"/>
       <c r="L36" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>31</v>
       </c>
       <c r="M36" s="7" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">41, </v>
       </c>
       <c r="N36" s="18" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">255
 </v>
       </c>
       <c r="O36" s="18"/>
-      <c r="P36" s="22"/>
+      <c r="P36" s="23"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
@@ -2411,40 +2414,40 @@
       <c r="M37" s="7"/>
       <c r="N37" s="18"/>
       <c r="O37" s="18"/>
-      <c r="P37" s="22"/>
+      <c r="P37" s="23"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
       <c r="C38" s="7"/>
       <c r="O38" s="18"/>
-      <c r="P38" s="22"/>
+      <c r="P38" s="23"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B39" s="3"/>
       <c r="C39" s="7"/>
       <c r="H39" s="6"/>
       <c r="O39" s="18"/>
-      <c r="P39" s="22"/>
+      <c r="P39" s="23"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C40" s="7"/>
       <c r="H40" s="6"/>
       <c r="O40" s="18"/>
-      <c r="P40" s="22"/>
+      <c r="P40" s="23"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="H41" s="6"/>
       <c r="O41" s="18"/>
-      <c r="P41" s="22"/>
+      <c r="P41" s="23"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="H42" s="6"/>
       <c r="O42" s="18"/>
-      <c r="P42" s="22"/>
+      <c r="P42" s="23"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="O43" s="18"/>
-      <c r="P43" s="22"/>
+      <c r="P43" s="23"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="O44" s="6"/>

</xml_diff>

<commit_message>
Add RID name generation to LUT generator
</commit_message>
<xml_diff>
--- a/lut_generator_rid.xlsx
+++ b/lut_generator_rid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shared\Dokumente\codebase\avr-rid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B815C9AF-E09C-4F92-97D5-BA012690DF83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F080E3F3-567D-4BA3-B5C2-1E40FD3662D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10690" yWindow="0" windowWidth="36500" windowHeight="18320" xr2:uid="{F31E432E-1247-4F18-8B99-AC2EE1672703}"/>
   </bookViews>
@@ -790,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52672B51-097A-4F0D-94C8-36FB4DE8AA5D}">
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F5:F35"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="L67" sqref="L67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -805,7 +805,7 @@
     <col min="6" max="11" width="11.08984375" customWidth="1"/>
     <col min="12" max="12" width="11.08984375" style="6" customWidth="1"/>
     <col min="13" max="14" width="11.08984375" customWidth="1"/>
-    <col min="15" max="15" width="2.81640625" customWidth="1"/>
+    <col min="15" max="15" width="11.90625" customWidth="1"/>
     <col min="16" max="16" width="59.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -926,7 +926,10 @@
         <f t="shared" ref="N5:N33" si="1">IF(J5&lt;&gt;"",J5-1&amp;", "&amp;IF($H5&lt;&gt;$H6,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
         <v xml:space="preserve">20, </v>
       </c>
-      <c r="O5" s="18"/>
+      <c r="O5" s="6" t="str">
+        <f>"RID_"&amp;FLOOR($E5/1000,1)&amp;"K"&amp;IF($E5&lt;10000,MOD($E5,1000)/100,"")&amp;","</f>
+        <v>RID_0K0,</v>
+      </c>
       <c r="P5" s="22" t="str">
         <f>"const __flash uint"&amp;$C$8*8&amp;"_t "&amp;"lut"&amp;$C$7*8&amp;"_"&amp;$C$6&amp;"["&amp;COUNT($J:$J)+1+COUNT($L:$L)&amp;"] ="&amp;CHAR(10)&amp;"{"&amp;CHAR(10)&amp;_xlfn.CONCAT($M:$M)&amp;CHAR(10)&amp;CHAR(10)&amp;_xlfn.CONCAT($N:$N)&amp;"};"</f>
         <v>const __flash uint8_t lut16_rid[42] =
@@ -994,7 +997,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">38, </v>
       </c>
-      <c r="O6" s="18"/>
+      <c r="O6" s="6" t="str">
+        <f t="shared" ref="O6:O35" si="8">"RID_"&amp;FLOOR($E6/1000,1)&amp;"K"&amp;IF($E6&lt;10000,MOD($E6,1000)/100,"")&amp;","</f>
+        <v>RID_1K0,</v>
+      </c>
       <c r="P6" s="23"/>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1044,7 +1050,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">57, </v>
       </c>
-      <c r="O7" s="18"/>
+      <c r="O7" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_1K5,</v>
+      </c>
       <c r="P7" s="23"/>
     </row>
     <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1094,7 +1103,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">87, </v>
       </c>
-      <c r="O8" s="18"/>
+      <c r="O8" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_2K2,</v>
+      </c>
       <c r="P8" s="23"/>
     </row>
     <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1144,7 +1156,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">126, </v>
       </c>
-      <c r="O9" s="18"/>
+      <c r="O9" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_3K3,</v>
+      </c>
       <c r="P9" s="23"/>
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1179,7 +1194,7 @@
         <v>3.1722806180047858E-3</v>
       </c>
       <c r="L10" s="6" t="str">
-        <f t="shared" ref="L10:L33" si="8">IF($H9&lt;&gt;$H10,ROW($H10)-ROW($H$5),"")</f>
+        <f t="shared" ref="L10:L33" si="9">IF($H9&lt;&gt;$H10,ROW($H10)-ROW($H$5),"")</f>
         <v/>
       </c>
       <c r="M10" s="7" t="str">
@@ -1190,7 +1205,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">155, </v>
       </c>
-      <c r="O10" s="18"/>
+      <c r="O10" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_4K7,</v>
+      </c>
       <c r="P10" s="23"/>
     </row>
     <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1225,7 +1243,7 @@
         <v>-2.2218079291056458E-3</v>
       </c>
       <c r="L11" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M11" s="7" t="str">
@@ -1236,7 +1254,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">189, </v>
       </c>
-      <c r="O11" s="18"/>
+      <c r="O11" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_5K6,</v>
+      </c>
       <c r="P11" s="23"/>
     </row>
     <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1273,7 +1294,7 @@
         <v>6.6453960302026438E-4</v>
       </c>
       <c r="L12" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M12" s="7" t="str">
@@ -1285,7 +1306,10 @@
         <v xml:space="preserve">228, 
 </v>
       </c>
-      <c r="O12" s="18"/>
+      <c r="O12" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_6K8,</v>
+      </c>
       <c r="P12" s="23"/>
     </row>
     <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1325,7 +1349,7 @@
         <v>-3.2629605114934401E-3</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="M13" s="7" t="str">
@@ -1336,7 +1360,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">139, </v>
       </c>
-      <c r="O13" s="18"/>
+      <c r="O13" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_8K2,</v>
+      </c>
       <c r="P13" s="23"/>
     </row>
     <row r="14" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1371,7 +1398,7 @@
         <v>5.159770764739946E-4</v>
       </c>
       <c r="L14" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M14" s="7" t="str">
@@ -1382,7 +1409,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">167, </v>
       </c>
-      <c r="O14" s="18"/>
+      <c r="O14" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_10K,</v>
+      </c>
       <c r="P14" s="23"/>
     </row>
     <row r="15" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1419,7 +1449,7 @@
         <v>-2.079552652477501E-3</v>
       </c>
       <c r="L15" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M15" s="7" t="str">
@@ -1430,7 +1460,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">208, </v>
       </c>
-      <c r="O15" s="18"/>
+      <c r="O15" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_12K,</v>
+      </c>
       <c r="P15" s="23"/>
     </row>
     <row r="16" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1483,7 +1516,7 @@
         <v>1.4819366044493965E-3</v>
       </c>
       <c r="L16" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M16" s="7" t="str">
@@ -1495,7 +1528,10 @@
         <v xml:space="preserve">251, 
 </v>
       </c>
-      <c r="O16" s="18"/>
+      <c r="O16" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_15K,</v>
+      </c>
       <c r="P16" s="23"/>
     </row>
     <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1530,7 +1566,7 @@
         <v>-1.857823774236711E-3</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="M17" s="7" t="str">
@@ -1541,7 +1577,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">153, </v>
       </c>
-      <c r="O17" s="18"/>
+      <c r="O17" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_18K,</v>
+      </c>
       <c r="P17" s="23"/>
     </row>
     <row r="18" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1576,7 +1615,7 @@
         <v>-2.5113299836080349E-3</v>
       </c>
       <c r="L18" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M18" s="7" t="str">
@@ -1587,7 +1626,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">188, </v>
       </c>
-      <c r="O18" s="18"/>
+      <c r="O18" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_22K,</v>
+      </c>
       <c r="P18" s="23"/>
     </row>
     <row r="19" spans="1:16" s="2" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1622,7 +1664,7 @@
         <v>-1.6392758804441021E-3</v>
       </c>
       <c r="L19" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M19" s="7" t="str">
@@ -1634,7 +1676,10 @@
         <v xml:space="preserve">230, 
 </v>
       </c>
-      <c r="O19" s="18"/>
+      <c r="O19" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_27K,</v>
+      </c>
       <c r="P19" s="23"/>
     </row>
     <row r="20" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1669,7 +1714,7 @@
         <v>1.406502170509194E-3</v>
       </c>
       <c r="L20" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="M20" s="7" t="str">
@@ -1680,7 +1725,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">136, </v>
       </c>
-      <c r="O20" s="18"/>
+      <c r="O20" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_33K,</v>
+      </c>
       <c r="P20" s="23"/>
     </row>
     <row r="21" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1715,7 +1763,7 @@
         <v>-1.9743950142470101E-3</v>
       </c>
       <c r="L21" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M21" s="7" t="str">
@@ -1726,7 +1774,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">164, </v>
       </c>
-      <c r="O21" s="18"/>
+      <c r="O21" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_39K,</v>
+      </c>
       <c r="P21" s="23"/>
     </row>
     <row r="22" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1761,7 +1812,7 @@
         <v>-1.8995895415149233E-3</v>
       </c>
       <c r="L22" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M22" s="7" t="str">
@@ -1772,7 +1823,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">196, </v>
       </c>
-      <c r="O22" s="18"/>
+      <c r="O22" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_47K,</v>
+      </c>
       <c r="P22" s="23"/>
     </row>
     <row r="23" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1807,7 +1861,7 @@
         <v>-9.1273618873444207E-4</v>
       </c>
       <c r="L23" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M23" s="7" t="str">
@@ -1819,7 +1873,10 @@
         <v xml:space="preserve">237, 
 </v>
       </c>
-      <c r="O23" s="18"/>
+      <c r="O23" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_56K,</v>
+      </c>
       <c r="P23" s="23"/>
     </row>
     <row r="24" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1854,7 +1911,7 @@
         <v>-3.3414939357011564E-3</v>
       </c>
       <c r="L24" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="M24" s="7" t="str">
@@ -1865,7 +1922,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">143, </v>
       </c>
-      <c r="O24" s="18"/>
+      <c r="O24" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_68K,</v>
+      </c>
       <c r="P24" s="23"/>
     </row>
     <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1900,7 +1960,7 @@
         <v>-2.6642445201634501E-3</v>
       </c>
       <c r="L25" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M25" s="7" t="str">
@@ -1911,7 +1971,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">174, </v>
       </c>
-      <c r="O25" s="18"/>
+      <c r="O25" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_82K,</v>
+      </c>
       <c r="P25" s="23"/>
     </row>
     <row r="26" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1946,7 +2009,7 @@
         <v>4.0190141681328839E-5</v>
       </c>
       <c r="L26" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M26" s="7" t="str">
@@ -1958,7 +2021,10 @@
         <v xml:space="preserve">209, 
 </v>
       </c>
-      <c r="O26" s="18"/>
+      <c r="O26" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_100K,</v>
+      </c>
       <c r="P26" s="23"/>
     </row>
     <row r="27" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1993,7 +2059,7 @@
         <v>2.8123048728900812E-4</v>
       </c>
       <c r="L27" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="M27" s="7" t="str">
@@ -2004,7 +2070,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">129, </v>
       </c>
-      <c r="O27" s="18"/>
+      <c r="O27" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_120K,</v>
+      </c>
       <c r="P27" s="23"/>
     </row>
     <row r="28" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2039,7 +2108,7 @@
         <v>1.3961265691024849E-3</v>
       </c>
       <c r="L28" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M28" s="7" t="str">
@@ -2050,7 +2119,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">156, </v>
       </c>
-      <c r="O28" s="18"/>
+      <c r="O28" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_150K,</v>
+      </c>
       <c r="P28" s="23"/>
     </row>
     <row r="29" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2085,7 +2157,7 @@
         <v>1.0169075510590986E-3</v>
       </c>
       <c r="L29" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M29" s="7" t="str">
@@ -2096,7 +2168,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">190, </v>
       </c>
-      <c r="O29" s="18"/>
+      <c r="O29" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_180K,</v>
+      </c>
       <c r="P29" s="23"/>
     </row>
     <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2131,7 +2206,7 @@
         <v>3.405193521368588E-4</v>
       </c>
       <c r="L30" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M30" s="7" t="str">
@@ -2143,7 +2218,10 @@
         <v xml:space="preserve">233, 
 </v>
       </c>
-      <c r="O30" s="18"/>
+      <c r="O30" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_220K,</v>
+      </c>
       <c r="P30" s="23"/>
     </row>
     <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2178,7 +2256,7 @@
         <v>-6.8759502340853818E-4</v>
       </c>
       <c r="L31" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>26</v>
       </c>
       <c r="M31" s="7" t="str">
@@ -2189,7 +2267,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">142, </v>
       </c>
-      <c r="O31" s="18"/>
+      <c r="O31" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_270K,</v>
+      </c>
       <c r="P31" s="23"/>
     </row>
     <row r="32" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2224,7 +2305,7 @@
         <v>-4.1227007067767829E-5</v>
       </c>
       <c r="L32" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M32" s="7" t="str">
@@ -2236,7 +2317,10 @@
         <v xml:space="preserve">195, 
 </v>
       </c>
-      <c r="O32" s="18"/>
+      <c r="O32" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_330K,</v>
+      </c>
       <c r="P32" s="23"/>
     </row>
     <row r="33" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2271,7 +2355,7 @@
         <v>2.4943955472618295E-3</v>
       </c>
       <c r="L33" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>28</v>
       </c>
       <c r="M33" s="7" t="str">
@@ -2282,7 +2366,10 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">139, </v>
       </c>
-      <c r="O33" s="18"/>
+      <c r="O33" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_470K,</v>
+      </c>
       <c r="P33" s="23"/>
       <c r="R33" s="19"/>
     </row>
@@ -2318,19 +2405,22 @@
         <v>-1.8385226224488793E-3</v>
       </c>
       <c r="L34" s="6" t="str">
-        <f t="shared" ref="L34:L36" si="9">IF($H33&lt;&gt;$H34,ROW($H34)-ROW($H$5),"")</f>
+        <f t="shared" ref="L34:L36" si="10">IF($H33&lt;&gt;$H34,ROW($H34)-ROW($H$5),"")</f>
         <v/>
       </c>
       <c r="M34" s="7" t="str">
-        <f t="shared" ref="M34:M36" si="10">IF(L34&lt;&gt;"",L34+COUNT(L:L)&amp;", ","")</f>
+        <f t="shared" ref="M34:M36" si="11">IF(L34&lt;&gt;"",L34+COUNT(L:L)&amp;", ","")</f>
         <v/>
       </c>
       <c r="N34" s="18" t="str">
-        <f t="shared" ref="N34:N36" si="11">IF(J34&lt;&gt;"",J34-1&amp;", "&amp;IF($H34&lt;&gt;$H35,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
+        <f t="shared" ref="N34:N36" si="12">IF(J34&lt;&gt;"",J34-1&amp;", "&amp;IF($H34&lt;&gt;$H35,CHAR(10),""),256^$C$8-1&amp;CHAR(10))</f>
         <v xml:space="preserve">203, 
 </v>
       </c>
-      <c r="O34" s="18"/>
+      <c r="O34" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_680K,</v>
+      </c>
       <c r="P34" s="23"/>
     </row>
     <row r="35" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2365,19 +2455,22 @@
         <v>1.5281238070927738E-3</v>
       </c>
       <c r="L35" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="M35" s="7" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">40, </v>
       </c>
       <c r="N35" s="18" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">169, 
 </v>
       </c>
-      <c r="O35" s="18"/>
+      <c r="O35" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>RID_1000K,</v>
+      </c>
       <c r="P35" s="23"/>
     </row>
     <row r="36" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2393,15 +2486,15 @@
       <c r="J36"/>
       <c r="K36"/>
       <c r="L36" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="M36" s="7" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">41, </v>
       </c>
       <c r="N36" s="18" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">255
 </v>
       </c>
@@ -2436,27 +2529,156 @@
       <c r="P40" s="23"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="H41" s="6"/>
+      <c r="E41" s="20"/>
       <c r="O41" s="18"/>
       <c r="P41" s="23"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="H42" s="6"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
       <c r="O42" s="18"/>
       <c r="P42" s="23"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E43" s="20"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
       <c r="O43" s="18"/>
       <c r="P43" s="23"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E44" s="20"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
       <c r="O44" s="6"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E45" s="20"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
       <c r="O45" s="6"/>
     </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E46" s="20"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E47" s="20"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+    </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="E48" s="20"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
       <c r="O48" s="6"/>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E49" s="20"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E50" s="20"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E51" s="20"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E52" s="20"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E53" s="20"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E54" s="20"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E55" s="20"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E56" s="20"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E57" s="20"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E58" s="20"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E59" s="20"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E60" s="20"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+    </row>
+    <row r="61" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E61" s="20"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E62" s="20"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E63" s="20"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E64" s="20"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E65" s="20"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E66" s="20"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E67" s="20"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E68" s="20"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E69" s="20"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
     </row>
   </sheetData>
   <sortState ref="E5">

</xml_diff>